<commit_message>
fixed signs on water quality parameters
</commit_message>
<xml_diff>
--- a/parameter_files/de_dg_gwq_upper.xlsx
+++ b/parameter_files/de_dg_gwq_upper.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4efc3e9dc81381f4/Documents/SJV-gen-modeling/parameter_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{1B55F186-EA2C-4865-8DAB-A5C1B6051DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05F59547-BF21-4057-A36B-902BA3CE50D4}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{1B55F186-EA2C-4865-8DAB-A5C1B6051DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F34C23C-2EB5-472A-9AE7-39A30E92EB95}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C11508F3-0935-47AB-A4FD-BF724EA4D517}"/>
   </bookViews>
@@ -674,7 +674,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J7" sqref="J7"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -685,19 +685,19 @@
     <row r="1" spans="1:8" s="14" customFormat="1" ht="76" x14ac:dyDescent="0.35">
       <c r="A1" s="11"/>
       <c r="B1" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>3</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>4</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>5</v>
@@ -765,22 +765,20 @@
       <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="4">
-        <v>-1</v>
-      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="4">
         <v>-1</v>
       </c>
@@ -790,16 +788,16 @@
       <c r="E8" s="4">
         <v>-1</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="4">
+        <v>-1</v>
+      </c>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="4">
-        <v>-1</v>
-      </c>
+      <c r="B9" s="2"/>
       <c r="C9" s="4">
         <v>-1</v>
       </c>
@@ -809,7 +807,9 @@
       <c r="E9" s="4">
         <v>-1</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="4">
+        <v>-1</v>
+      </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -904,22 +904,20 @@
       <c r="A18" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="2">
-        <v>2</v>
-      </c>
+      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="8">
-        <v>-1</v>
-      </c>
+      <c r="B19" s="3"/>
       <c r="C19" s="8">
         <v>-1</v>
       </c>
@@ -929,16 +927,16 @@
       <c r="E19" s="8">
         <v>-1</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="8">
+        <v>-1</v>
+      </c>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="8">
-        <v>-1</v>
-      </c>
+      <c r="B20" s="2"/>
       <c r="C20" s="8">
         <v>-1</v>
       </c>
@@ -948,40 +946,40 @@
       <c r="E20" s="8">
         <v>-1</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="8">
+        <v>-1</v>
+      </c>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="3"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
+      <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="3">
+        <v>2</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="3">
-        <v>2</v>
-      </c>
+      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="4">
-        <v>-1</v>
-      </c>
+      <c r="B23" s="4"/>
       <c r="C23" s="4">
         <v>-1</v>
       </c>
@@ -991,7 +989,9 @@
       <c r="E23" s="4">
         <v>-1</v>
       </c>
-      <c r="F23" s="4"/>
+      <c r="F23" s="4">
+        <v>-1</v>
+      </c>
       <c r="G23" s="4">
         <v>-1</v>
       </c>
@@ -1025,9 +1025,7 @@
       <c r="A26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="4">
-        <v>-1</v>
-      </c>
+      <c r="B26" s="2"/>
       <c r="C26" s="4">
         <v>-1</v>
       </c>
@@ -1037,16 +1035,16 @@
       <c r="E26" s="4">
         <v>-1</v>
       </c>
-      <c r="F26" s="2"/>
+      <c r="F26" s="4">
+        <v>-1</v>
+      </c>
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="4">
-        <v>-1</v>
-      </c>
+      <c r="B27" s="2"/>
       <c r="C27" s="4">
         <v>-1</v>
       </c>
@@ -1056,16 +1054,16 @@
       <c r="E27" s="4">
         <v>-1</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="4">
+        <v>-1</v>
+      </c>
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:8" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="4">
-        <v>-1</v>
-      </c>
+      <c r="B28" s="2"/>
       <c r="C28" s="4">
         <v>-1</v>
       </c>
@@ -1075,7 +1073,9 @@
       <c r="E28" s="4">
         <v>-1</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="4">
+        <v>-1</v>
+      </c>
       <c r="G28" s="2"/>
     </row>
   </sheetData>

</xml_diff>